<commit_message>
create matriz  product and espTec
</commit_message>
<xml_diff>
--- a/ProductoPlavaVea.xlsx
+++ b/ProductoPlavaVea.xlsx
@@ -8,18 +8,28 @@
   </bookViews>
   <sheets>
     <sheet name="PRODUCTO" sheetId="1" r:id="rId1"/>
+    <sheet name="ESP_TECNICAS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>01000101</t>
   </si>
   <si>
-    <t>0001</t>
+    <t>MEGIMPERU</t>
+  </si>
+  <si>
+    <t>Gancho Organizador para Reposacabezas de Asiento</t>
+  </si>
+  <si>
+    <t>TOP GAN</t>
+  </si>
+  <si>
+    <t>Piso para Auto TOP GAM Negro</t>
   </si>
   <si>
     <t>Tipo</t>
@@ -399,50 +409,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -455,17 +489,17 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -478,17 +512,17 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -501,17 +535,17 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -524,17 +558,17 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -547,17 +581,17 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -570,17 +604,17 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -590,49 +624,26 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add all products to excel
</commit_message>
<xml_diff>
--- a/ProductoPlavaVea.xlsx
+++ b/ProductoPlavaVea.xlsx
@@ -8,28 +8,174 @@
   </bookViews>
   <sheets>
     <sheet name="PRODUCTO" sheetId="1" r:id="rId1"/>
-    <sheet name="ESP_TECNICAS" sheetId="2" r:id="rId2"/>
+    <sheet name="OTRADESC" sheetId="2" r:id="rId2"/>
+    <sheet name="ESP_TECNICAS" sheetId="3" r:id="rId3"/>
+    <sheet name="PRODUCTO-EMPRESA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="93">
   <si>
     <t>01000101</t>
   </si>
   <si>
+    <t>Gancho Organizador para Reposacabezas de Asiento</t>
+  </si>
+  <si>
     <t>MEGIMPERU</t>
   </si>
   <si>
-    <t>Gancho Organizador para Reposacabezas de Asiento</t>
+    <t>Piso para Auto TOP GAM Negro</t>
   </si>
   <si>
     <t>TOP GAN</t>
   </si>
   <si>
-    <t>Piso para Auto TOP GAM Negro</t>
+    <t>Red de carga 91.44x121.92cm con 12 ganchos</t>
+  </si>
+  <si>
+    <t>MINTCRAFT</t>
+  </si>
+  <si>
+    <t>Funda de timón para automóvil Azul</t>
+  </si>
+  <si>
+    <t>SPARCO</t>
+  </si>
+  <si>
+    <t>Kit para cambio de llantas</t>
+  </si>
+  <si>
+    <t>BARRON VIEYRA</t>
+  </si>
+  <si>
+    <t>Set 4 cubrepisos para auto goma y alfombra</t>
+  </si>
+  <si>
+    <t>GOODYEAR</t>
+  </si>
+  <si>
+    <t>Cojín lumbar</t>
+  </si>
+  <si>
+    <t>PROMART</t>
+  </si>
+  <si>
+    <t>Respaldo anatómico Lumbar Cushion</t>
+  </si>
+  <si>
+    <t>Asiento para automóvil</t>
+  </si>
+  <si>
+    <t>FOAMFLEX</t>
+  </si>
+  <si>
+    <t>Asiento de automóvil para niño</t>
+  </si>
+  <si>
+    <t>Limpiaparabrisas 26"</t>
+  </si>
+  <si>
+    <t>BOSCH</t>
+  </si>
+  <si>
+    <t>Limpiaparabrisas 24"</t>
+  </si>
+  <si>
+    <t>Cepillo Limpiaparabrisas ECO 14"</t>
+  </si>
+  <si>
+    <t>Limpiador renovador de llantas 500 ml</t>
+  </si>
+  <si>
+    <t>SIMONIZ</t>
+  </si>
+  <si>
+    <t>Barra de bloqueo 60066</t>
+  </si>
+  <si>
+    <t>Tapones regulares para pitón x4 unidades</t>
+  </si>
+  <si>
+    <t>ITW GLOBAL BRANDS</t>
+  </si>
+  <si>
+    <t>Tapones cromados para pitón x4 unidades</t>
+  </si>
+  <si>
+    <t>Medidor de aire doble cabeza</t>
+  </si>
+  <si>
+    <t>Medidor digital de neumático Slime</t>
+  </si>
+  <si>
+    <t>Kit de parchado de llanta Slime</t>
+  </si>
+  <si>
+    <t>Gancho Organizador Para Reposacabezas del Asiento del Auto---------- Haga que su coche se vea ordenado y limpio.--------- Convierte el reposacabezas de tu coche en un conveniente espacio de almacenamiento para colgar alimentos, ropa, paraguas, bolsos, botellas de agua, juguetes, objetos del bebé y mucho más.----------- Su especial diseño, mitad abierto, permite instalar estos ganchos fácilmente, sin necesidad de quitar el reposacabezas del vehículo, puedes libremente fijar o quitar los ganchos en segundos sin herramientas adicionales, de forma rápida y práctica.-------------- Ahorro de espacio con el gancho organizador de asiento trasero del auto que se coloca en el reposacabezas con el cual donde podrá organiza bolsas de mano, bolsos de mano, monederos, bolsas de escuela, paraguas y más.--------- Características:---------- Universal apto para la mayoría de los coches, furgonetas, camionetas y SUVs------------- Material: ABS-------------- Diseño especial para fácil instalación.-------------- Organiza bolsas de mano, bolsos de mano, mochilas, paraguas y más-------------- 11cm x 10cm x 6cm-------------- Carga máxima total: 3 kg-------------- Color Negro-------------- Paquete incluido: 1 gancho de doble percha</t>
+  </si>
+  <si>
+    <t>./</t>
+  </si>
+  <si>
+    <t>Foto y descripción referencial</t>
+  </si>
+  <si>
+    <t>plazaVea, presenta una línea de accesorios de seguridad para el automóvil, con una calidad Premium. Reúne los mejores e innovadores productos para su disposición. Las redes son la sujeción perfecta para amarrar la carga en motocicletas, coches, bicicletas, camiones, embarcaciones, remolques, etc. Este elemento es de gran utilidad para sujetar bien el equipaje en el coche, por ejemplo, en vacaciones. Los ganchos de los extremos aseguran la estabilidad de la carga.</t>
+  </si>
+  <si>
+    <t>Hecho de un resistente material a base poliuretano y caucho, lo que asegura un mejor agarre al conducir y protección a la superficie del timón; adaptable a timones de 38 cm x 8.2 cm, garantizando su perfecta adhesión a la forma. Definitivamente, un producto que velará por el buen mantenimiento de su automóvil y añadirá valor estético al mismo.</t>
+  </si>
+  <si>
+    <t>plazaVea, presenta una línea de accesorios de seguridad para el automóvil, con una calidad Premium. Reúne los mejores e innovadores productos para su disposición. Cambiar las llantas de un auto es relativamente fácil, solo se necesitan las herramientas adecuadas para que todo el trabajo resulte a la perfección. Te ofrecemos, este kit para cambiar neumáticos, que contiene todos los implementos necesarios. Las herramientas para cambiar las llantas de un auto son: destornilladores, llaves, linternas, entre otras.</t>
+  </si>
+  <si>
+    <t>Ideal para proteger el interior del auto de la suciedad generada por el polvo y/o barro.</t>
+  </si>
+  <si>
+    <t>Este cojín lumbar de Foamflex se coloca en el espaldar del asiento de tu auto u oficina. Este te ayuda a tener una mejor postura mientras te sientas, previniendo problemas de espalda o columna posteriores. Es perfecto para personas que vayan a pasar largo tiempo sentados. Por ejemplo, mientras manejan o trabajan.</t>
+  </si>
+  <si>
+    <t>Este respaldar anatómico de Foamflex se coloca en la espalda del asiento que vayas a usar. Este te ayuda a tener una mejor postura mientras te sientas, previniendo problemas de espalda o columna posteriores. Es perfecto para personas que vayan a pasar largo tiempo sentados. Por ejemplo, mientras manejan, ven televisión o trabajan.</t>
+  </si>
+  <si>
+    <t>Este asiento para auto de Foamflex es ideal para un viaje mucho más seguro, ya que permite una mejor visión del camino, a la vez que da mayor comodidad al usuario. Solo asegúrate de que la persona esté sentada correctamente y bien segura.</t>
+  </si>
+  <si>
+    <t>Este asiento booster para niños de Foamflex es ideal para un uso correcto del cinturón de seguridad, ya que ayuda a que los brazos de los pequeños se apoyen mejor y de forma cómoda, a la vez que les permite una mejor visión del camino mientras pasean en carro. También, es perfecto para darles mayor altura en otros lugares como el cine, restaurantes y más.</t>
+  </si>
+  <si>
+    <t>plazaVea y Hobby Pro traen las mejores cuerdas para ti. La driza de poliéster está específicamente concebida para uso en exteriores, ya que soporta perfectamente las inclemencias del tiempo, no se pudre y es resistente a los rayos UV. Alta resistencia a la abrasión y a las rupturas. No dejes de comprar este útil producto en plazaVea.</t>
+  </si>
+  <si>
+    <t>Bosch y plazaVea se unen para brindarte los mejores accesorios para tus herramientas eléctricas. Ya seas un profesional de la construcción o no, tus trabajos quedarán impecables gracias a la excelente calidad de los productos que esta marca alemana te ofrece. Hoy trae un limpiaparabrisas que te garantiza una performance idónea aún en condiciones climáticas extremas. Gracias a este obtendrás la mejor visibilidad y disfrutarás de un viaje seguro. Lleva hoy tu limpiaparabrisas Bosch, la mejor marca en la categoría. ¡Encuéntralo en plazaVea!</t>
+  </si>
+  <si>
+    <t>Bosch y plazaVea se unen para brindarte los mejores accesorios para tus vehículos. Tus lunas quedarán impecables gracias a la excelente performance y calidad de los productos que esta marca alemana te ofrece. Hoy trae el cepillo limpiaparabrisas ECO de 14 pulgadas con diseño aerodinámico, compuesto de caucho natural y recubrimiento de grafito, por lo cual no se oxida. Puede mejorar su desempeño en altas velocidades. Es muy fácil de colocar. Engríe tu auto con este grandioso producto. ¡Encuentra los mejores productos en plazaVea!</t>
+  </si>
+  <si>
+    <t>plazaVea le recomienda el cuidado y mantenimiento eficiente de su vehículo, por tanto presenta el Limpiador renovador de llantas Simoniz. Limpia, cuida y protege los neumáticos de los vehículos con una sola pasada. Simplemente rociar sobre las ruedas y pasar un paño seco suavemente. Limpia hasta los neumáticos más sucios, le devuelve el profundo brillo y el color a los que estén desmoronados. Mantiene el cucho suave y lo protege contra las grietas y quebradiza.</t>
+  </si>
+  <si>
+    <t>Goodyear y plazaVea se unen para ofrecerte la mejor calidad de productos en accesorios de seguridad para tu vehículo. La barra de bloqueo, es ideal para asegurar tu automóvil y evitar robos. ¡Con la calidad y seguridad que solo Goodyear te ofrece!</t>
+  </si>
+  <si>
+    <t>Slime es líder mundial en productos para el cuidado de los neumáticos. Ahora plazaVea te ofrece su amplia variedad de productos destinados a satisfacer las necesidades según el problema que se preste. Los tapones de Slime están diseñados para cerrar o asegurar la entrada de la válvula de las llanta de autos y motos. Son resistentes, durables y capaces de adaptarse a todo tipo de pitón o entrada de válvula de un neumático. Puedes llevarlo en este paquete de 4 unidades.</t>
+  </si>
+  <si>
+    <t>plazaVea te brinda una calidad superior en artículos de automotriz, para que tu vehículo tenga un recorrido sin inconvenientes. Los tapones cromados para pitón, son ideales para impedir la salida de aire de las llantas de tu auto y así evites accidentes. ¡Con la confianza y seguridad que te ofrecen los productos de plazaVea!</t>
+  </si>
+  <si>
+    <t>Las mejores herramientas para tu auto las consigues con Truper. En esta oportunidad te ofrece un medidor de aire de cabeza doble para válvulas con difícil acceso. Posee un largo de 14.5 centímetros y un rango de 10-120 PSI. Es de gran durabilidad ya que el cuerpo es de latón, cabezas metálicas y la regleta de aluminio. Es muy fácil al usarlo, colócalo en la válvula y la regleta saldrá indicando la presión que tienen las llantas.</t>
+  </si>
+  <si>
+    <t>Mide la presión de tus neumáticos con este medidor digital Slime de 0-120 psi, que te hace la tarea mucho más fácil y rápida. Podrás comprobar de forma segura el inflado de las llantas de tu vehículo.</t>
+  </si>
+  <si>
+    <t>Este kit es perfecto para reparar pinchaduras de llanta al instante. Solo necesitas colocar el líquido sobre el hueco que quieras reparar y dejar secar rápidamente. También sirve para prevenir, así que es ideal para usar antes de un paseo largo.</t>
   </si>
   <si>
     <t>Tipo</t>
@@ -78,6 +224,79 @@
   </si>
   <si>
     <t>1 gancho de doble percha</t>
+  </si>
+  <si>
+    <t>Regular
+S/ 45.00</t>
+  </si>
+  <si>
+    <t>S/ 19.99</t>
+  </si>
+  <si>
+    <t>-55%</t>
+  </si>
+  <si>
+    <t>20532584681</t>
+  </si>
+  <si>
+    <t>PLAZA VEA</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>MegimPeru</t>
+  </si>
+  <si>
+    <t>S/ 82.90</t>
+  </si>
+  <si>
+    <t>S/ 61.90</t>
+  </si>
+  <si>
+    <t>S/ 44.90</t>
+  </si>
+  <si>
+    <t>S/ 21.90</t>
+  </si>
+  <si>
+    <t>S/ 69.90</t>
+  </si>
+  <si>
+    <t>S/ 26.90</t>
+  </si>
+  <si>
+    <t>S/ 34.90</t>
+  </si>
+  <si>
+    <t>S/ 29.90</t>
+  </si>
+  <si>
+    <t>S/ 22.90</t>
+  </si>
+  <si>
+    <t>S/ 20.90</t>
+  </si>
+  <si>
+    <t>S/ 14.90</t>
+  </si>
+  <si>
+    <t>S/ 24.90</t>
+  </si>
+  <si>
+    <t>S/ 6.90</t>
+  </si>
+  <si>
+    <t>S/ 10.90</t>
+  </si>
+  <si>
+    <t>S/ 41.90</t>
+  </si>
+  <si>
+    <t>S/ 57.90</t>
+  </si>
+  <si>
+    <t>S/ 28.90</t>
   </si>
 </sst>
 </file>
@@ -409,7 +628,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,12 +668,611 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G9"/>
   <sheetViews>
@@ -473,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -496,10 +1314,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -519,10 +1337,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -542,10 +1360,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -565,10 +1383,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -588,10 +1406,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -611,10 +1429,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -634,15 +1452,911 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
         <v>1</v>
       </c>
     </row>

</xml_diff>